<commit_message>
Changed example to match our data input expectations
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonorato\Documents\DIRECT Classes\Alaska_Project\ACEP_solar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDE96F57-BA2A-4539-A87D-E32651B57C75}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C241CE7-47CA-4678-A589-B4234D7DC4AA}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{0283CA11-9A3F-4AE3-9A17-25FFC6E80EDE}"/>
   </bookViews>
@@ -87,7 +87,7 @@
     <t>Juneau</t>
   </si>
   <si>
-    <t>Interpolated</t>
+    <t>Interpolate</t>
   </si>
 </sst>
 </file>
@@ -442,7 +442,7 @@
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>